<commit_message>
Change date and format submitter info clearly
</commit_message>
<xml_diff>
--- a/docs/docs/gencc-submission-sheet-v1.xlsx
+++ b/docs/docs/gencc-submission-sheet-v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottg/SitesDev/gencc-website/docs/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2488588E-5440-8E41-9031-61BD17F0E636}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C75046-670C-B34D-85D5-A6EC1B5125B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>OPTIONAL - Text string of the MOI. The submitted text won't be displayed publically on the website. Information provided will primarily be used to support audit/review.</t>
   </si>
   <si>
-    <t>REQUIRED - The date should be provided as ISO8601.</t>
-  </si>
-  <si>
     <t>RECOMMENDED BUT OPTIONAL - If available, the full url to where a visitor can access a public report/information (not in GenCC)</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>Autosomal dominant inheritance</t>
   </si>
   <si>
-    <t>00001</t>
-  </si>
-  <si>
     <t>Lab123 Corp</t>
   </si>
   <si>
@@ -182,9 +176,6 @@
   </si>
   <si>
     <t>Definitive</t>
-  </si>
-  <si>
-    <t>2020-01-28T16:22:37-0700</t>
   </si>
   <si>
     <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit. Mauris blandit, justo eu mollis finibus, eros elit efficitur eros, sed tincidunt quam ipsum ac felis. </t>
@@ -431,6 +422,15 @@
   </si>
   <si>
     <t>The GenCC website required MOI to be provided as HPO terms.  The following are suggested common MOI identifiers. When sharing submissions, please ensure that the classification_id column contains one of the following identifiers (HP:XXXXXX).</t>
+  </si>
+  <si>
+    <t>2020/01/20</t>
+  </si>
+  <si>
+    <t>REQUIRED - The date should be provided as YYYY/MM/DD</t>
+  </si>
+  <si>
+    <t>GENCC:10001</t>
   </si>
 </sst>
 </file>
@@ -940,7 +940,9 @@
   </sheetPr>
   <dimension ref="A1:AD1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1089,7 +1091,7 @@
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="42" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1168,7 +1170,7 @@
         <v>18</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -1208,31 +1210,31 @@
         <v>25</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L7" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="M7" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="N7" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="O7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="17" t="s">
-        <v>29</v>
-      </c>
       <c r="P7" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Q7" s="21"/>
       <c r="R7" s="21"/>
@@ -1251,7 +1253,7 @@
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -1285,96 +1287,96 @@
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="C9" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="D9" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="E9" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="F9" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="G9" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="H9" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="I9" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="J9" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="K9" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="31" t="s">
-        <v>41</v>
-      </c>
       <c r="L9" s="32" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="M9" s="33"/>
       <c r="N9" s="34" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O9" s="35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P9" s="36" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q9" s="37"/>
       <c r="R9" s="37"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="E10" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="F10" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="M10" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="31" t="s">
+      <c r="N10" s="34" t="s">
         <v>40</v>
-      </c>
-      <c r="K10" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="L10" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="N10" s="34" t="s">
-        <v>43</v>
       </c>
       <c r="O10" s="35"/>
       <c r="P10" s="38"/>
@@ -1383,55 +1385,55 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="31" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="H11" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="J11" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="K11" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="31" t="s">
-        <v>41</v>
-      </c>
       <c r="L11" s="32" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="M11" s="33" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="N11" s="34"/>
       <c r="O11" s="35" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="P11" s="39" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q11" s="37"/>
       <c r="R11" s="37"/>
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -21349,12 +21351,12 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A1" s="44" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -21396,106 +21398,106 @@
     </row>
     <row r="4" spans="1:30" ht="14" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
         <v>60</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>64</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
         <v>66</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
         <v>68</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
         <v>72</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
         <v>74</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
         <v>76</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
         <v>78</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
         <v>80</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
         <v>82</v>
-      </c>
-      <c r="B15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -21519,12 +21521,12 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A1" s="44" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -21566,74 +21568,74 @@
     </row>
     <row r="4" spans="1:30" ht="14" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>86</v>
       </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>87</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>89</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
         <v>91</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
         <v>93</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
         <v>95</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
         <v>97</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
         <v>99</v>
-      </c>
-      <c r="B11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -21657,12 +21659,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="44" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B2" s="7"/>
     </row>
@@ -21676,58 +21678,58 @@
     </row>
     <row r="4" spans="1:2" ht="14" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
         <v>112</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>114</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
         <v>116</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
         <v>118</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
         <v>120</v>
-      </c>
-      <c r="B9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>